<commit_message>
Inserindo argumento que faltou para não salvar o index nos arquivos xlsx
</commit_message>
<xml_diff>
--- a/dados_tratados/inscricao_2022.xlsx
+++ b/dados_tratados/inscricao_2022.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,397 +434,340 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Subscription Date</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>48</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Brady</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brady</t>
+          <t>mccalltyrone@durham-rose.biz</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mccalltyrone@durham-rose.biz</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>2022-03-10</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>63</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Chloe</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Chloe</t>
+          <t>leah85@sutton-terrell.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>leah85@sutton-terrell.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>2022-05-15</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>26</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dakota</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dakota</t>
+          <t>stacey67@fields.org</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>stacey67@fields.org</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
           <t>2022-02-20</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>94</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Darrell</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Darrell</t>
+          <t>grayjean@lowery-good.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>grayjean@lowery-good.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
           <t>2022-02-17</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>62</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Eddie</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Eddie</t>
+          <t>kristiwhitney@bernard.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>kristiwhitney@bernard.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
           <t>2022-03-24</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>85</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Emma</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>walter83@juarez.org</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>walter83@juarez.org</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
           <t>2022-05-13</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>14</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Faith</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Faith</t>
+          <t>cassieparrish@blevins-chapman.net</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>cassieparrish@blevins-chapman.net</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
           <t>2022-01-26</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>27</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Frederick</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Frederick</t>
+          <t>jacobkhan@bright.biz</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>jacobkhan@bright.biz</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
           <t>2022-05-26</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>47</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gloria</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gloria</t>
+          <t>bartlettjenna@zuniga-moss.biz</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>bartlettjenna@zuniga-moss.biz</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
           <t>2022-03-11</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>17</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Greg</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>jaredjuarez@carroll.org</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>jaredjuarez@carroll.org</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
           <t>2022-03-26</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>95</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Karl</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Karl</t>
+          <t>hhart@jensen.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>hhart@jensen.com</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
           <t>2022-01-30</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>43</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Luis</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>bstuart@williamson-mcclure.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>bstuart@williamson-mcclure.com</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
           <t>2022-05-15</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>25</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Marcus</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>donnamullins@norris-barrett.org</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>donnamullins@norris-barrett.org</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
           <t>2022-05-24</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>20</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Maxwell</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Maxwell</t>
+          <t>fgibson@drake-webb.com</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fgibson@drake-webb.com</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
           <t>2022-01-12</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>15</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Miranda</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Miranda</t>
+          <t>vduncan@parks-hardy.com</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>vduncan@parks-hardy.com</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
           <t>2022-04-12</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>74</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>zrosario@rojas-hardin.net</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>zrosario@rojas-hardin.net</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
           <t>2022-01-15</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>54</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Robin</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Robin</t>
+          <t>greenemiranda@zimmerman.com</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>greenemiranda@zimmerman.com</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
           <t>2022-01-13</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>35</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tammie</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tammie</t>
+          <t>harrisisaiah@jenkins.com</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>harrisisaiah@jenkins.com</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
           <t>2022-01-04</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>31</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Tom</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>tapiagreg@beard.info</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
-        <is>
-          <t>tapiagreg@beard.info</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
         <is>
           <t>2022-01-13</t>
         </is>

</xml_diff>